<commit_message>
Made visual and legend interactive.
</commit_message>
<xml_diff>
--- a/documents/Published/Venn Diagram/VennDiagramByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Venn Diagram/VennDiagramByMAQSoftwareChecklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Power BI\VennDiagram\14-9-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\documents\Published\Venn Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>S no</t>
   </si>
@@ -279,6 +279,30 @@
   </si>
   <si>
     <t>iPad - yes</t>
+  </si>
+  <si>
+    <t>Legend Interactivity</t>
+  </si>
+  <si>
+    <t>Click on Legend value.</t>
+  </si>
+  <si>
+    <t>Data should get filtered on clicking particular legend value. Also opacity should get changed for the circle accordingly.</t>
+  </si>
+  <si>
+    <t>Check whether Legend is interactive.</t>
+  </si>
+  <si>
+    <t>Visual Interactivity</t>
+  </si>
+  <si>
+    <t>Check whether Visual is interactive.</t>
+  </si>
+  <si>
+    <t>Data should get filtered for the "Maths" category. Also opacity should get changed for that circle accordingly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on "Maths"  path element(circle).                          [NOTE : For overlapping(Intersection) path elements there is no interactivity]                               </t>
   </si>
 </sst>
 </file>
@@ -735,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD02BEF-CDC7-45AE-AEC8-BFE8DA79D8E7}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,6 +878,40 @@
       </c>
       <c r="E7" s="4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Legend and Visual interactive.
</commit_message>
<xml_diff>
--- a/documents/Published/Venn Diagram/VennDiagramByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/Venn Diagram/VennDiagramByMAQSoftwareChecklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Power BI\VennDiagram\14-9-17\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\documents\Published\Venn Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>S no</t>
   </si>
@@ -279,6 +279,30 @@
   </si>
   <si>
     <t>iPad - yes</t>
+  </si>
+  <si>
+    <t>Legend Interactivity</t>
+  </si>
+  <si>
+    <t>Click on Legend value.</t>
+  </si>
+  <si>
+    <t>Data should get filtered on clicking particular legend value. Also opacity should get changed for the circle accordingly.</t>
+  </si>
+  <si>
+    <t>Check whether Legend is interactive.</t>
+  </si>
+  <si>
+    <t>Visual Interactivity</t>
+  </si>
+  <si>
+    <t>Check whether Visual is interactive.</t>
+  </si>
+  <si>
+    <t>Data should get filtered for the "Maths" category. Also opacity should get changed for that circle accordingly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on "Maths"  path element(circle).                          [NOTE : For overlapping(Intersection) path elements there is no interactivity]                               </t>
   </si>
 </sst>
 </file>
@@ -735,10 +759,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECD02BEF-CDC7-45AE-AEC8-BFE8DA79D8E7}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,6 +878,40 @@
       </c>
       <c r="E7" s="4" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>